<commit_message>
criada a classe Obj
</commit_message>
<xml_diff>
--- a/documentacao/bakclog.xlsx
+++ b/documentacao/bakclog.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\prog2\formula1_novo\documentacao\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\prog2\arthur_dev3\formula1_novo\documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -847,8 +847,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -896,7 +896,7 @@
       <c r="B3" t="s">
         <v>49</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>